<commit_message>
adding commit of excel format in case of deletion
</commit_message>
<xml_diff>
--- a/Master/PyBudget_master.xlsx
+++ b/Master/PyBudget_master.xlsx
@@ -9,20 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7515" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7515" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Debit Data" sheetId="1" r:id="rId1"/>
     <sheet name="Credit Data" sheetId="2" r:id="rId2"/>
-    <sheet name="YTD" sheetId="3" r:id="rId3"/>
+    <sheet name="Jan" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="master" localSheetId="1" hidden="1">'Credit Data'!$F$1:$J$128</definedName>
     <definedName name="master_1" localSheetId="1" hidden="1">'Credit Data'!$M$8:$Q$135</definedName>
-    <definedName name="PyBudget_data" localSheetId="1" hidden="1">'Credit Data'!$A$1:$E$28</definedName>
+    <definedName name="PyBudget_data" localSheetId="1" hidden="1">'Credit Data'!$A$1:$E$21</definedName>
     <definedName name="PyBudget_data" localSheetId="0" hidden="1">'Debit Data'!$A$1:$E$128</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="191">
   <si>
     <t>Date</t>
   </si>
@@ -427,18 +427,6 @@
     <t>E TFR   C0hWhPnE</t>
   </si>
   <si>
-    <t>food</t>
-  </si>
-  <si>
-    <t>transfer</t>
-  </si>
-  <si>
-    <t>fof</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
     <t>COMPASS VENDING</t>
   </si>
   <si>
@@ -482,13 +470,161 @@
   </si>
   <si>
     <t>INTEREST CHARGE -PURCHASE</t>
+  </si>
+  <si>
+    <t>alcohol</t>
+  </si>
+  <si>
+    <t>groceries</t>
+  </si>
+  <si>
+    <t>dining</t>
+  </si>
+  <si>
+    <t>credit transfer</t>
+  </si>
+  <si>
+    <t>hobbies</t>
+  </si>
+  <si>
+    <t>clothing</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>01/01/2017</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>Spendings</t>
+  </si>
+  <si>
+    <t>Debit</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Groceries</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>01/12/2017</t>
+  </si>
+  <si>
+    <t>WESTJET     8382122368434</t>
+  </si>
+  <si>
+    <t>NEW LEAF</t>
+  </si>
+  <si>
+    <t>01/15/2017</t>
+  </si>
+  <si>
+    <t>IMPARK00011888U</t>
+  </si>
+  <si>
+    <t>PAYMENT - THANK YOU</t>
+  </si>
+  <si>
+    <t>KOODO AIRTIME</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>UNIVERSITY OF ALBERTA</t>
+  </si>
+  <si>
+    <t>01/30/2017</t>
+  </si>
+  <si>
+    <t>02/02/2017</t>
+  </si>
+  <si>
+    <t>UNIVERSITY OF ALBERTA ORS</t>
+  </si>
+  <si>
+    <t>Rent</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Tuition</t>
+  </si>
+  <si>
+    <t>Vacation</t>
+  </si>
+  <si>
+    <t>Alcohol</t>
+  </si>
+  <si>
+    <t>Dining</t>
+  </si>
+  <si>
+    <t>Hobbies</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>Exercise</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Need</t>
+  </si>
+  <si>
+    <t>Want</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Total Spendings</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,14 +650,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -551,6 +704,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Overall</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -564,7 +742,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -583,193 +761,153 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="19050">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="lt1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:marker>
-          <c:yVal>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-0FD6-4D4F-8FDE-C79985D1C52C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-0FD6-4D4F-8FDE-C79985D1C52C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Jan!$B$4,Jan!$B$6)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Income</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spendings</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>YTD!$E$6:$E$8</c:f>
+              <c:f>(Jan!$C$4,Jan!$C$6)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>8451.7799999999988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>7821.17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-192D-4432-ABB4-0DDFCD09BAB8}"/>
+              <c16:uniqueId val="{00000000-0FD6-4D4F-8FDE-C79985D1C52C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:axId val="364276192"/>
-        <c:axId val="364273568"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="364276192"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="364273568"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="364273568"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="364276192"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -778,6 +916,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -802,7 +971,295 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Percent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> Saved</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Jan!$B$4:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Income</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Savings</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Jan!$C$4:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>8451.7799999999988</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>630.60999999999876</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1313-4143-9EDA-0FA50F24A79A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -855,8 +1312,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -883,8 +1380,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -913,7 +1410,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -964,6 +1461,13 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -974,18 +1478,25 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1020,7 +1531,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1341,17 +1852,525 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1375,23 +2394,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50D6D113-2AB7-4DEF-B1B1-A0125EBCFC60}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9807F96E-F8EC-4ECE-8905-52397C28267F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1404,6 +2423,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BF835FB-CA49-4287-B007-7FE4AD96EA09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1455,8 +2510,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_PyBudget_data3" displayName="Table_PyBudget_data3" ref="A1:E28" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_PyBudget_data3" displayName="Table_PyBudget_data3" ref="A1:E21" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:E21"/>
   <tableColumns count="5">
     <tableColumn id="1" uniqueName="1" name="Date" queryTableFieldId="2"/>
     <tableColumn id="2" uniqueName="2" name="Transaction" queryTableFieldId="3"/>
@@ -1755,7 +2810,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="E212" sqref="E212"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1796,7 +2853,7 @@
         <v>12893.09</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1813,7 +2870,7 @@
         <v>12804.14</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1830,7 +2887,7 @@
         <v>12761.62</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1847,7 +2904,7 @@
         <v>12736.77</v>
       </c>
       <c r="E5" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1864,7 +2921,7 @@
         <v>12731.02</v>
       </c>
       <c r="E6" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1898,7 +2955,7 @@
         <v>12656.76</v>
       </c>
       <c r="E8" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1915,7 +2972,7 @@
         <v>12636.76</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1966,7 +3023,7 @@
         <v>12696.26</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1983,7 +3040,7 @@
         <v>12691.55</v>
       </c>
       <c r="E13" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2119,7 +3176,7 @@
         <v>13442.43</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2136,7 +3193,7 @@
         <v>13432.15</v>
       </c>
       <c r="E22" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2170,7 +3227,7 @@
         <v>13399.9</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2204,7 +3261,7 @@
         <v>13110.15</v>
       </c>
       <c r="E26" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2221,7 +3278,7 @@
         <v>13104.9</v>
       </c>
       <c r="E27" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2238,7 +3295,7 @@
         <v>12990.45</v>
       </c>
       <c r="E28" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2255,7 +3312,7 @@
         <v>12988.57</v>
       </c>
       <c r="E29" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2323,7 +3380,7 @@
         <v>12574.82</v>
       </c>
       <c r="E33" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2408,7 +3465,7 @@
         <v>13711.82</v>
       </c>
       <c r="E38" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2442,7 +3499,7 @@
         <v>13694.11</v>
       </c>
       <c r="E40" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2476,7 +3533,7 @@
         <v>13445.23</v>
       </c>
       <c r="E42" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2487,7 +3544,7 @@
         <v>57</v>
       </c>
       <c r="C43">
-        <v>-1800</v>
+        <v>-900</v>
       </c>
       <c r="D43">
         <v>11645.23</v>
@@ -2521,13 +3578,13 @@
         <v>59</v>
       </c>
       <c r="C45">
-        <v>654.79999999999995</v>
+        <v>-254.2</v>
       </c>
       <c r="D45">
         <v>12299.03</v>
       </c>
       <c r="E45" t="s">
-        <v>58</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2629,7 +3686,7 @@
         <v>13981.49</v>
       </c>
       <c r="E51" t="s">
-        <v>26</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2646,7 +3703,7 @@
         <v>13909.04</v>
       </c>
       <c r="E52" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2680,7 +3737,7 @@
         <v>13727.85</v>
       </c>
       <c r="E54" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2697,7 +3754,7 @@
         <v>13714.41</v>
       </c>
       <c r="E55" t="s">
-        <v>16</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2748,7 +3805,7 @@
         <v>13653.44</v>
       </c>
       <c r="E58" t="s">
-        <v>26</v>
+        <v>144</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2765,7 +3822,7 @@
         <v>13632.44</v>
       </c>
       <c r="E59" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2782,7 +3839,7 @@
         <v>13622.79</v>
       </c>
       <c r="E60" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2850,7 +3907,7 @@
         <v>14836.83</v>
       </c>
       <c r="E64" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2901,7 +3958,7 @@
         <v>14754.24</v>
       </c>
       <c r="E67" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2918,7 +3975,7 @@
         <v>14729.13</v>
       </c>
       <c r="E68" t="s">
-        <v>26</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2935,7 +3992,7 @@
         <v>14721.88</v>
       </c>
       <c r="E69" t="s">
-        <v>26</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2952,7 +4009,7 @@
         <v>14703.99</v>
       </c>
       <c r="E70" t="s">
-        <v>26</v>
+        <v>144</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2969,7 +4026,7 @@
         <v>14695.94</v>
       </c>
       <c r="E71" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2986,7 +4043,7 @@
         <v>14672.13</v>
       </c>
       <c r="E72" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3003,7 +4060,7 @@
         <v>14669.03</v>
       </c>
       <c r="E73" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3020,7 +4077,7 @@
         <v>14664.42</v>
       </c>
       <c r="E74" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3037,7 +4094,7 @@
         <v>14601.9</v>
       </c>
       <c r="E75" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3173,7 +4230,7 @@
         <v>13675.84</v>
       </c>
       <c r="E83" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3224,7 +4281,7 @@
         <v>14614.16</v>
       </c>
       <c r="E86" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3241,7 +4298,7 @@
         <v>14582.26</v>
       </c>
       <c r="E87" t="s">
-        <v>26</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3292,7 +4349,7 @@
         <v>14571.4</v>
       </c>
       <c r="E90" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3309,7 +4366,7 @@
         <v>14447.2</v>
       </c>
       <c r="E91" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3360,7 +4417,7 @@
         <v>13301.66</v>
       </c>
       <c r="E94" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3428,7 +4485,7 @@
         <v>13228</v>
       </c>
       <c r="E98" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3479,7 +4536,7 @@
         <v>13213.76</v>
       </c>
       <c r="E101" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3496,7 +4553,7 @@
         <v>13199.21</v>
       </c>
       <c r="E102" t="s">
-        <v>26</v>
+        <v>148</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3513,7 +4570,7 @@
         <v>13122.38</v>
       </c>
       <c r="E103" t="s">
-        <v>26</v>
+        <v>148</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3547,7 +4604,7 @@
         <v>13112.62</v>
       </c>
       <c r="E105" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3581,7 +4638,7 @@
         <v>14786.6</v>
       </c>
       <c r="E107" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3632,7 +4689,7 @@
         <v>14755.43</v>
       </c>
       <c r="E110" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3666,7 +4723,7 @@
         <v>14625.86</v>
       </c>
       <c r="E112" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3700,7 +4757,7 @@
         <v>14572.29</v>
       </c>
       <c r="E114" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3717,7 +4774,7 @@
         <v>14495.45</v>
       </c>
       <c r="E115" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3751,7 +4808,7 @@
         <v>14424.46</v>
       </c>
       <c r="E117" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3785,7 +4842,7 @@
         <v>14319.46</v>
       </c>
       <c r="E119" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3819,7 +4876,7 @@
         <v>14307.15</v>
       </c>
       <c r="E121" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3853,7 +4910,7 @@
         <v>13406.15</v>
       </c>
       <c r="E123" t="s">
-        <v>132</v>
+        <v>58</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -3951,10 +5008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3993,118 +5050,118 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="C2">
-        <v>-106</v>
+        <v>-145.03</v>
       </c>
       <c r="D2">
-        <v>168.34</v>
+        <v>289.8</v>
       </c>
       <c r="E2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3">
+        <v>-89</v>
+      </c>
+      <c r="D3">
+        <v>378.8</v>
+      </c>
+      <c r="E3" t="s">
         <v>135</v>
-      </c>
-      <c r="B3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C3">
-        <v>-13.38</v>
-      </c>
-      <c r="D3">
-        <v>181.72</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="C4">
-        <v>-18</v>
+        <v>-2</v>
       </c>
       <c r="D4">
-        <v>199.72</v>
+        <v>380.8</v>
       </c>
       <c r="E4" t="s">
-        <v>139</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="C5">
-        <v>-56.69</v>
+        <v>380.8</v>
       </c>
       <c r="D5">
-        <v>256.41000000000003</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="C6">
-        <v>-16.7</v>
+        <v>-197.88</v>
       </c>
       <c r="D6">
-        <v>273.11</v>
+        <v>197.88</v>
       </c>
       <c r="E6" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="C7">
-        <v>-16.7</v>
+        <v>-50</v>
       </c>
       <c r="D7">
-        <v>289.81</v>
+        <v>247.88</v>
       </c>
       <c r="E7" t="s">
-        <v>139</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C8">
         <v>-9.99</v>
       </c>
       <c r="D8">
-        <v>299.8</v>
+        <v>257.87</v>
       </c>
       <c r="E8" t="s">
         <v>26</v>
@@ -4112,33 +5169,33 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="C9">
-        <v>-2.84</v>
+        <v>247.88</v>
       </c>
       <c r="D9">
-        <v>302.64</v>
+        <v>9.99</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>170</v>
       </c>
       <c r="B10" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="C10">
-        <v>-3.41</v>
+        <v>-50</v>
       </c>
       <c r="D10">
-        <v>306.05</v>
+        <v>59.99</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
@@ -4149,7 +5206,7 @@
         <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C11">
         <v>-106</v>
@@ -4158,295 +5215,176 @@
         <v>168.34</v>
       </c>
       <c r="E11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C12">
-        <v>-13.38</v>
+        <v>-2.29</v>
       </c>
       <c r="D12">
-        <v>181.72</v>
+        <v>62.28</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C13">
-        <v>-18</v>
+        <v>-0.06</v>
       </c>
       <c r="D13">
-        <v>199.72</v>
+        <v>62.34</v>
       </c>
       <c r="E13" t="s">
-        <v>139</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C14">
-        <v>-56.69</v>
+        <v>-13.38</v>
       </c>
       <c r="D14">
-        <v>256.41000000000003</v>
+        <v>181.72</v>
       </c>
       <c r="E14" t="s">
-        <v>142</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C15">
-        <v>-16.7</v>
+        <v>-18</v>
       </c>
       <c r="D15">
-        <v>273.11</v>
+        <v>199.72</v>
       </c>
       <c r="E15" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C16">
-        <v>-16.7</v>
+        <v>-56.69</v>
       </c>
       <c r="D16">
-        <v>289.81</v>
+        <v>256.41000000000003</v>
       </c>
       <c r="E16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C17">
-        <v>-9.99</v>
+        <v>-16.7</v>
       </c>
       <c r="D17">
-        <v>299.8</v>
+        <v>273.11</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C18">
-        <v>-2.84</v>
+        <v>-16.7</v>
       </c>
       <c r="D18">
-        <v>302.64</v>
+        <v>289.81</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C19">
-        <v>-3.41</v>
+        <v>-9.99</v>
       </c>
       <c r="D19">
-        <v>306.05</v>
+        <v>299.8</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="B20" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="C20">
-        <v>-106</v>
+        <v>-2.84</v>
       </c>
       <c r="D20">
-        <v>168.34</v>
+        <v>302.64</v>
       </c>
       <c r="E20" t="s">
-        <v>134</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="B21" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C21">
-        <v>-13.38</v>
+        <v>-3.41</v>
       </c>
       <c r="D21">
-        <v>181.72</v>
+        <v>306.05</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>137</v>
-      </c>
-      <c r="B22" t="s">
-        <v>138</v>
-      </c>
-      <c r="C22">
-        <v>-18</v>
-      </c>
-      <c r="D22">
-        <v>199.72</v>
-      </c>
-      <c r="E22" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" t="s">
-        <v>141</v>
-      </c>
-      <c r="C23">
-        <v>-56.69</v>
-      </c>
-      <c r="D23">
-        <v>256.41000000000003</v>
-      </c>
-      <c r="E23" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C24">
-        <v>-16.7</v>
-      </c>
-      <c r="D24">
-        <v>273.11</v>
-      </c>
-      <c r="E24" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" t="s">
-        <v>144</v>
-      </c>
-      <c r="C25">
-        <v>-16.7</v>
-      </c>
-      <c r="D25">
-        <v>289.81</v>
-      </c>
-      <c r="E25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>89</v>
-      </c>
-      <c r="B26" t="s">
-        <v>145</v>
-      </c>
-      <c r="C26">
-        <v>-9.99</v>
-      </c>
-      <c r="D26">
-        <v>299.8</v>
-      </c>
-      <c r="E26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>95</v>
-      </c>
-      <c r="B27" t="s">
-        <v>146</v>
-      </c>
-      <c r="C27">
-        <v>-2.84</v>
-      </c>
-      <c r="D27">
-        <v>302.64</v>
-      </c>
-      <c r="E27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C28">
-        <v>-3.41</v>
-      </c>
-      <c r="D28">
-        <v>306.05</v>
-      </c>
-      <c r="E28" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4460,30 +5398,517 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E6:E8"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="6" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E8">
-        <v>3</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="1">
+        <f>SUMIFS('Debit Data'!C2:C1000,'Debit Data'!E2:E1000, B4, 'Debit Data'!A2:A1000, "&gt;"&amp;$B$1)</f>
+        <v>8451.7799999999988</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="1">
+        <f>C4-C6</f>
+        <v>630.60999999999876</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="1">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, "&lt;&gt;income",'Debit Data'!$E$2:$E$1000, "&lt;&gt;credit transfer",'Debit Data'!$E$2:$E$1000, "&lt;&gt;savings transfer", 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2) - SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, "&lt;&gt;income",'Credit Data'!$E$2:$E$1000, "&lt;&gt;credit transfer",'Credit Data'!$E$2:$E$1000, "&lt;&gt;savings transfer", 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>7821.17</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="1">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B10, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>822.86999999999989</v>
+      </c>
+      <c r="D10" s="1">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B10, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <f>SUM(C10:D10)</f>
+        <v>822.86999999999989</v>
+      </c>
+      <c r="F10" s="4">
+        <f>E10/$C$36</f>
+        <v>0.10521060148289832</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="2">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B11, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B11, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>197.88</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" ref="E11:E31" si="0">SUM(C11:D11)</f>
+        <v>197.88</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" ref="F11:F31" si="1">E11/$C$36</f>
+        <v>2.530056244781791E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="2">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B12, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>2700</v>
+      </c>
+      <c r="D12" s="2">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B12, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>2700</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.3452168921018211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C13" s="2">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B13, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>284.08</v>
+      </c>
+      <c r="D13" s="2">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B13, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>284.08</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="1"/>
+        <v>3.6321931373439011E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C14" s="2">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B14, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>222.75</v>
+      </c>
+      <c r="D14" s="2">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B14, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>222.75</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="1"/>
+        <v>2.8480393598400239E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C15" s="2">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B15, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>1075.24</v>
+      </c>
+      <c r="D15" s="2">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B15, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>1075.24</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="1"/>
+        <v>0.13747815224576374</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" s="1">
+        <f>SUM(C10:C15)</f>
+        <v>5104.9399999999996</v>
+      </c>
+      <c r="D17" s="1">
+        <f>SUM(D10:D15)</f>
+        <v>197.88</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>5302.82</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="1"/>
+        <v>0.67800853325014032</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" s="1">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B21, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>475</v>
+      </c>
+      <c r="D21" s="1">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B21, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>285.43</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>760.43000000000006</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="1"/>
+        <v>9.7227141207773274E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="2">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B22, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>181.51</v>
+      </c>
+      <c r="D22" s="2">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B22, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
+        <v>181.51</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="1"/>
+        <v>2.3207525216815385E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C23" s="2">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B23, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>184.51000000000002</v>
+      </c>
+      <c r="D23" s="2">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B23, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>184.51000000000002</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" si="1"/>
+        <v>2.3591099541372968E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24" s="2">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B24, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>91.38</v>
+      </c>
+      <c r="D24" s="2">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B24, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="0"/>
+        <v>91.38</v>
+      </c>
+      <c r="F24" s="4">
+        <f t="shared" si="1"/>
+        <v>1.1683673926023855E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C25" s="2">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B25, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>69.989999999999995</v>
+      </c>
+      <c r="D25" s="2">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B25, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="0"/>
+        <v>69.989999999999995</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="1"/>
+        <v>8.9487889919283164E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" s="2">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B26, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>724.67000000000007</v>
+      </c>
+      <c r="D26" s="2">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B26, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>56.69</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="0"/>
+        <v>781.36000000000013</v>
+      </c>
+      <c r="F26" s="4">
+        <f t="shared" si="1"/>
+        <v>9.9903211412103315E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C27" s="2">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B27, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B27, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>106</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" ref="E27" si="2">SUM(C27:D27)</f>
+        <v>106</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="1"/>
+        <v>1.3552959467701124E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C28" s="2">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B28, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>45.39</v>
+      </c>
+      <c r="D28" s="2">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B28, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>33.36</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="0"/>
+        <v>78.75</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="1"/>
+        <v>1.0068826019636448E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C29" s="2">
+        <f>-SUMIFS('Debit Data'!$C$2:$C$1000,'Debit Data'!$E$2:$E$1000, B29, 'Debit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1,'Debit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>153.82</v>
+      </c>
+      <c r="D29" s="2">
+        <f>-SUMIFS('Credit Data'!$C$2:$C$1000,'Credit Data'!$E$2:$E$1000, B29, 'Credit Data'!$A$2:$A$1000, "&gt;="&amp;$B$1, 'Credit Data'!$A$2:$A$1000, "&lt;="&amp;$B$2)</f>
+        <v>110.60000000000001</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" ref="E29" si="3">SUM(C29:D29)</f>
+        <v>264.42</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" si="1"/>
+        <v>3.3808240966505011E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C31" s="1">
+        <f>SUM(C21:C29)</f>
+        <v>1926.27</v>
+      </c>
+      <c r="D31" s="1">
+        <f>SUM(D21:D29)</f>
+        <v>592.08000000000004</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="0"/>
+        <v>2518.35</v>
+      </c>
+      <c r="F31" s="4">
+        <f t="shared" si="1"/>
+        <v>0.32199146674985968</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="1">
+        <f>SUM(C31,C17)</f>
+        <v>7031.2099999999991</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" s="1">
+        <f>SUM(D17,D31)</f>
+        <v>789.96</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C36" s="1">
+        <f>SUM(E31,E17)</f>
+        <v>7821.17</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B19:F19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>